<commit_message>
fixed error in data, updated app appearance
</commit_message>
<xml_diff>
--- a/Baukastenstuecklisten.xlsx
+++ b/Baukastenstuecklisten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liria\Desktop\HiWi\testing\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA7BBF9-E93E-41E3-807D-D7B988089EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{485ABF9E-43E9-4ED4-B880-5E896E59DD56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12696" yWindow="-13068" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="142">
   <si>
     <t>Benennung:</t>
   </si>
@@ -323,9 +323,6 @@
 M4x10</t>
   </si>
   <si>
-    <t>BG 014</t>
-  </si>
-  <si>
     <t>BG Getriebe Fußgehäuse 4</t>
   </si>
   <si>
@@ -389,9 +386,6 @@
     <t>BG Klemmkasten</t>
   </si>
   <si>
-    <t>BG 021</t>
-  </si>
-  <si>
     <t>BG Asynchronmotor 1</t>
   </si>
   <si>
@@ -822,6 +816,9 @@
   <si>
     <t>Sechskantschrauben
 M4x15</t>
+  </si>
+  <si>
+    <t>BT 014</t>
   </si>
 </sst>
 </file>
@@ -1451,6 +1448,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1470,21 +1482,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1803,37 +1800,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82EB9C67-F2F5-44CE-AEE1-7EE413D5E386}">
   <dimension ref="A1:M139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
-      <selection activeCell="O64" sqref="O64"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="P91" sqref="P91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="60" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="59"/>
-      <c r="E1" s="60" t="s">
+      <c r="B1" s="64"/>
+      <c r="C1" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="64"/>
+      <c r="E1" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="61"/>
-      <c r="H1" s="58" t="s">
+      <c r="F1" s="66"/>
+      <c r="H1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="59"/>
-      <c r="J1" s="60" t="s">
+      <c r="I1" s="64"/>
+      <c r="J1" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="59"/>
-      <c r="L1" s="60" t="s">
+      <c r="K1" s="64"/>
+      <c r="L1" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="61"/>
+      <c r="M1" s="66"/>
     </row>
     <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
@@ -1951,31 +1948,31 @@
       <c r="G5" s="11"/>
     </row>
     <row r="6" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="58" t="s">
+      <c r="A6" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="59"/>
-      <c r="C6" s="60" t="s">
+      <c r="B6" s="64"/>
+      <c r="C6" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="59"/>
-      <c r="E6" s="60" t="s">
+      <c r="D6" s="64"/>
+      <c r="E6" s="65" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="61"/>
+      <c r="F6" s="66"/>
       <c r="G6" s="11"/>
-      <c r="H6" s="58" t="s">
+      <c r="H6" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="59"/>
-      <c r="J6" s="60" t="s">
+      <c r="I6" s="64"/>
+      <c r="J6" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="K6" s="59"/>
-      <c r="L6" s="60" t="s">
+      <c r="K6" s="64"/>
+      <c r="L6" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="M6" s="61"/>
+      <c r="M6" s="66"/>
     </row>
     <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="18" t="s">
@@ -2112,18 +2109,18 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="58" t="s">
+      <c r="A11" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="59"/>
-      <c r="C11" s="60" t="s">
+      <c r="B11" s="64"/>
+      <c r="C11" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="59"/>
-      <c r="E11" s="60" t="s">
+      <c r="D11" s="64"/>
+      <c r="E11" s="65" t="s">
         <v>60</v>
       </c>
-      <c r="F11" s="61"/>
+      <c r="F11" s="66"/>
       <c r="G11" s="11"/>
     </row>
     <row r="12" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2146,18 +2143,18 @@
         <v>10</v>
       </c>
       <c r="G12" s="11"/>
-      <c r="H12" s="58" t="s">
+      <c r="H12" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="I12" s="59"/>
-      <c r="J12" s="60" t="s">
+      <c r="I12" s="64"/>
+      <c r="J12" s="65" t="s">
         <v>51</v>
       </c>
-      <c r="K12" s="59"/>
-      <c r="L12" s="60" t="s">
+      <c r="K12" s="64"/>
+      <c r="L12" s="65" t="s">
         <v>62</v>
       </c>
-      <c r="M12" s="61"/>
+      <c r="M12" s="66"/>
     </row>
     <row r="13" spans="1:13" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="15">
@@ -2248,18 +2245,18 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="58" t="s">
+      <c r="A16" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="59"/>
-      <c r="C16" s="60" t="s">
+      <c r="B16" s="64"/>
+      <c r="C16" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="59"/>
-      <c r="E16" s="62" t="s">
+      <c r="D16" s="64"/>
+      <c r="E16" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="63"/>
+      <c r="F16" s="68"/>
     </row>
     <row r="17" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="18" t="s">
@@ -2280,18 +2277,18 @@
       <c r="F17" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="H17" s="58" t="s">
+      <c r="H17" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="I17" s="59"/>
-      <c r="J17" s="60" t="s">
+      <c r="I17" s="64"/>
+      <c r="J17" s="65" t="s">
         <v>55</v>
       </c>
-      <c r="K17" s="59"/>
-      <c r="L17" s="60" t="s">
-        <v>76</v>
-      </c>
-      <c r="M17" s="61"/>
+      <c r="K17" s="64"/>
+      <c r="L17" s="65" t="s">
+        <v>75</v>
+      </c>
+      <c r="M17" s="66"/>
     </row>
     <row r="18" spans="1:13" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="15">
@@ -2375,25 +2372,25 @@
         <v>16</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M20" s="3" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="58" t="s">
+      <c r="A21" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="59"/>
-      <c r="C21" s="60" t="s">
+      <c r="B21" s="64"/>
+      <c r="C21" s="65" t="s">
         <v>61</v>
       </c>
-      <c r="D21" s="59"/>
-      <c r="E21" s="62" t="s">
+      <c r="D21" s="64"/>
+      <c r="E21" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="F21" s="63"/>
+      <c r="F21" s="68"/>
       <c r="H21" s="9">
         <v>3</v>
       </c>
@@ -2449,18 +2446,18 @@
         <v>58</v>
       </c>
       <c r="G23" s="11"/>
-      <c r="H23" s="58" t="s">
+      <c r="H23" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="I23" s="59"/>
-      <c r="J23" s="60" t="s">
+      <c r="I23" s="64"/>
+      <c r="J23" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="K23" s="59"/>
-      <c r="L23" s="60" t="s">
-        <v>91</v>
-      </c>
-      <c r="M23" s="61"/>
+      <c r="K23" s="64"/>
+      <c r="L23" s="65" t="s">
+        <v>89</v>
+      </c>
+      <c r="M23" s="66"/>
     </row>
     <row r="24" spans="1:13" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="9">
@@ -2525,18 +2522,18 @@
       </c>
     </row>
     <row r="26" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="58" t="s">
+      <c r="A26" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="59"/>
-      <c r="C26" s="60" t="s">
+      <c r="B26" s="64"/>
+      <c r="C26" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="D26" s="59"/>
-      <c r="E26" s="60" t="s">
-        <v>96</v>
-      </c>
-      <c r="F26" s="61"/>
+      <c r="D26" s="64"/>
+      <c r="E26" s="65" t="s">
+        <v>94</v>
+      </c>
+      <c r="F26" s="66"/>
       <c r="G26" s="11"/>
       <c r="H26" s="2">
         <v>2</v>
@@ -2549,7 +2546,7 @@
         <v>16</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M26" s="24" t="s">
         <v>50</v>
@@ -2627,7 +2624,7 @@
         <v>16</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F29" s="24" t="s">
         <v>11</v>
@@ -2656,18 +2653,18 @@
         <v>12</v>
       </c>
       <c r="G30" s="11"/>
-      <c r="H30" s="58" t="s">
+      <c r="H30" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="I30" s="59"/>
-      <c r="J30" s="60" t="s">
-        <v>90</v>
-      </c>
-      <c r="K30" s="59"/>
-      <c r="L30" s="60" t="s">
-        <v>102</v>
-      </c>
-      <c r="M30" s="61"/>
+      <c r="I30" s="64"/>
+      <c r="J30" s="65" t="s">
+        <v>88</v>
+      </c>
+      <c r="K30" s="64"/>
+      <c r="L30" s="65" t="s">
+        <v>100</v>
+      </c>
+      <c r="M30" s="66"/>
     </row>
     <row r="31" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="11"/>
@@ -2697,18 +2694,18 @@
       </c>
     </row>
     <row r="32" spans="1:13" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="58" t="s">
+      <c r="A32" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="59"/>
-      <c r="C32" s="60" t="s">
+      <c r="B32" s="64"/>
+      <c r="C32" s="65" t="s">
         <v>63</v>
       </c>
-      <c r="D32" s="59"/>
-      <c r="E32" s="60" t="s">
-        <v>105</v>
-      </c>
-      <c r="F32" s="61"/>
+      <c r="D32" s="64"/>
+      <c r="E32" s="65" t="s">
+        <v>103</v>
+      </c>
+      <c r="F32" s="66"/>
       <c r="G32" s="11"/>
       <c r="H32" s="15">
         <v>1</v>
@@ -2721,10 +2718,10 @@
         <v>16</v>
       </c>
       <c r="L32" s="22" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="M32" s="25" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2758,10 +2755,10 @@
         <v>16</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M33" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -2793,10 +2790,10 @@
         <v>16</v>
       </c>
       <c r="L34" s="30" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M34" s="31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -2811,7 +2808,7 @@
         <v>16</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F35" s="24" t="s">
         <v>22</v>
@@ -2825,10 +2822,10 @@
       </c>
       <c r="K35" s="33"/>
       <c r="L35" s="34" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="M35" s="35" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -2851,30 +2848,30 @@
     </row>
     <row r="37" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="38" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="58" t="s">
+      <c r="A38" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="59"/>
-      <c r="C38" s="60" t="s">
+      <c r="B38" s="64"/>
+      <c r="C38" s="65" t="s">
         <v>67</v>
       </c>
-      <c r="D38" s="59"/>
-      <c r="E38" s="60" t="s">
-        <v>114</v>
-      </c>
-      <c r="F38" s="61"/>
-      <c r="H38" s="58" t="s">
+      <c r="D38" s="64"/>
+      <c r="E38" s="65" t="s">
+        <v>112</v>
+      </c>
+      <c r="F38" s="66"/>
+      <c r="H38" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="I38" s="59"/>
-      <c r="J38" s="60" t="s">
-        <v>92</v>
-      </c>
-      <c r="K38" s="59"/>
-      <c r="L38" s="60" t="s">
-        <v>115</v>
-      </c>
-      <c r="M38" s="61"/>
+      <c r="I38" s="64"/>
+      <c r="J38" s="65" t="s">
+        <v>90</v>
+      </c>
+      <c r="K38" s="64"/>
+      <c r="L38" s="65" t="s">
+        <v>113</v>
+      </c>
+      <c r="M38" s="66"/>
     </row>
     <row r="39" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="18" t="s">
@@ -2942,10 +2939,10 @@
         <v>16</v>
       </c>
       <c r="L40" s="22" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="M40" s="25" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
@@ -2960,7 +2957,7 @@
         <v>16</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F41" s="24" t="s">
         <v>30</v>
@@ -2976,10 +2973,10 @@
         <v>16</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M41" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -3010,10 +3007,10 @@
         <v>16</v>
       </c>
       <c r="L42" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M42" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3025,24 +3022,24 @@
       <c r="M43" s="36"/>
     </row>
     <row r="44" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="58" t="s">
+      <c r="A44" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="59"/>
-      <c r="C44" s="60" t="s">
-        <v>72</v>
-      </c>
-      <c r="D44" s="59"/>
-      <c r="E44" s="60" t="s">
-        <v>117</v>
-      </c>
-      <c r="F44" s="61"/>
-      <c r="H44" s="64"/>
-      <c r="I44" s="64"/>
-      <c r="J44" s="64"/>
-      <c r="K44" s="64"/>
-      <c r="L44" s="64"/>
-      <c r="M44" s="64"/>
+      <c r="B44" s="64"/>
+      <c r="C44" s="65" t="s">
+        <v>71</v>
+      </c>
+      <c r="D44" s="64"/>
+      <c r="E44" s="65" t="s">
+        <v>115</v>
+      </c>
+      <c r="F44" s="66"/>
+      <c r="H44" s="69"/>
+      <c r="I44" s="69"/>
+      <c r="J44" s="69"/>
+      <c r="K44" s="69"/>
+      <c r="L44" s="69"/>
+      <c r="M44" s="69"/>
     </row>
     <row r="45" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="18" t="s">
@@ -3087,18 +3084,18 @@
       <c r="F46" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="H46" s="58" t="s">
+      <c r="H46" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="I46" s="59"/>
-      <c r="J46" s="60" t="s">
-        <v>88</v>
-      </c>
-      <c r="K46" s="59"/>
-      <c r="L46" s="60" t="s">
-        <v>118</v>
-      </c>
-      <c r="M46" s="61"/>
+      <c r="I46" s="64"/>
+      <c r="J46" s="65" t="s">
+        <v>87</v>
+      </c>
+      <c r="K46" s="64"/>
+      <c r="L46" s="65" t="s">
+        <v>116</v>
+      </c>
+      <c r="M46" s="66"/>
     </row>
     <row r="47" spans="1:13" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
@@ -3112,7 +3109,7 @@
         <v>16</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F47" s="24" t="s">
         <v>37</v>
@@ -3164,10 +3161,10 @@
         <v>16</v>
       </c>
       <c r="L48" s="22" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="M48" s="25" t="s">
-        <v>71</v>
+        <v>141</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -3182,25 +3179,25 @@
         <v>16</v>
       </c>
       <c r="L49" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="M49" s="41" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="58" t="s">
+      <c r="A50" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="B50" s="59"/>
-      <c r="C50" s="60" t="s">
-        <v>73</v>
-      </c>
-      <c r="D50" s="59"/>
-      <c r="E50" s="60" t="s">
-        <v>122</v>
-      </c>
-      <c r="F50" s="61"/>
+      <c r="B50" s="64"/>
+      <c r="C50" s="65" t="s">
+        <v>72</v>
+      </c>
+      <c r="D50" s="64"/>
+      <c r="E50" s="65" t="s">
+        <v>120</v>
+      </c>
+      <c r="F50" s="66"/>
       <c r="H50" s="11"/>
       <c r="I50" s="57"/>
       <c r="J50" s="11"/>
@@ -3251,18 +3248,18 @@
       <c r="F52" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="H52" s="58" t="s">
+      <c r="H52" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="I52" s="59"/>
-      <c r="J52" s="60" t="s">
-        <v>94</v>
-      </c>
-      <c r="K52" s="59"/>
-      <c r="L52" s="60" t="s">
-        <v>123</v>
-      </c>
-      <c r="M52" s="61"/>
+      <c r="I52" s="64"/>
+      <c r="J52" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="K52" s="64"/>
+      <c r="L52" s="65" t="s">
+        <v>121</v>
+      </c>
+      <c r="M52" s="66"/>
     </row>
     <row r="53" spans="1:13" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="2">
@@ -3276,7 +3273,7 @@
         <v>16</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F53" s="24" t="s">
         <v>11</v>
@@ -3328,10 +3325,10 @@
         <v>16</v>
       </c>
       <c r="L54" s="22" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M54" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="55" spans="1:13" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -3359,18 +3356,18 @@
       </c>
     </row>
     <row r="56" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="58" t="s">
+      <c r="A56" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="B56" s="59"/>
-      <c r="C56" s="60" t="s">
-        <v>77</v>
-      </c>
-      <c r="D56" s="59"/>
-      <c r="E56" s="60" t="s">
-        <v>125</v>
-      </c>
-      <c r="F56" s="61"/>
+      <c r="B56" s="64"/>
+      <c r="C56" s="65" t="s">
+        <v>76</v>
+      </c>
+      <c r="D56" s="64"/>
+      <c r="E56" s="65" t="s">
+        <v>123</v>
+      </c>
+      <c r="F56" s="66"/>
     </row>
     <row r="57" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="18" t="s">
@@ -3409,18 +3406,18 @@
       <c r="F58" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="H58" s="58" t="s">
+      <c r="H58" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="I58" s="59"/>
-      <c r="J58" s="60" t="s">
-        <v>95</v>
-      </c>
-      <c r="K58" s="59"/>
-      <c r="L58" s="60" t="s">
-        <v>126</v>
-      </c>
-      <c r="M58" s="61"/>
+      <c r="I58" s="64"/>
+      <c r="J58" s="65" t="s">
+        <v>93</v>
+      </c>
+      <c r="K58" s="64"/>
+      <c r="L58" s="65" t="s">
+        <v>124</v>
+      </c>
+      <c r="M58" s="66"/>
     </row>
     <row r="59" spans="1:13" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="2">
@@ -3434,7 +3431,7 @@
         <v>16</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F59" s="24" t="s">
         <v>22</v>
@@ -3486,10 +3483,10 @@
         <v>16</v>
       </c>
       <c r="L60" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M60" s="25" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="61" spans="1:13" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -3504,25 +3501,25 @@
         <v>16</v>
       </c>
       <c r="L61" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="M61" s="24" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="62" spans="1:13" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="58" t="s">
+      <c r="A62" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="B62" s="59"/>
-      <c r="C62" s="60" t="s">
-        <v>79</v>
-      </c>
-      <c r="D62" s="59"/>
-      <c r="E62" s="60" t="s">
-        <v>127</v>
-      </c>
-      <c r="F62" s="61"/>
+      <c r="B62" s="64"/>
+      <c r="C62" s="65" t="s">
+        <v>78</v>
+      </c>
+      <c r="D62" s="64"/>
+      <c r="E62" s="65" t="s">
+        <v>125</v>
+      </c>
+      <c r="F62" s="66"/>
       <c r="G62" s="45"/>
       <c r="H62" s="43">
         <v>3</v>
@@ -3568,10 +3565,10 @@
         <v>16</v>
       </c>
       <c r="L63" s="49" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M63" s="26" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="64" spans="1:13" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -3604,23 +3601,23 @@
         <v>16</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F65" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="H65" s="58" t="s">
+      <c r="H65" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="I65" s="59"/>
-      <c r="J65" s="60" t="s">
-        <v>97</v>
-      </c>
-      <c r="K65" s="59"/>
-      <c r="L65" s="60" t="s">
-        <v>128</v>
-      </c>
-      <c r="M65" s="61"/>
+      <c r="I65" s="64"/>
+      <c r="J65" s="65" t="s">
+        <v>95</v>
+      </c>
+      <c r="K65" s="64"/>
+      <c r="L65" s="65" t="s">
+        <v>126</v>
+      </c>
+      <c r="M65" s="66"/>
     </row>
     <row r="66" spans="1:13" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="9">
@@ -3670,25 +3667,25 @@
         <v>16</v>
       </c>
       <c r="L67" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M67" s="25" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="68" spans="1:13" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="58" t="s">
+      <c r="A68" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="B68" s="59"/>
-      <c r="C68" s="60" t="s">
-        <v>82</v>
-      </c>
-      <c r="D68" s="59"/>
-      <c r="E68" s="60" t="s">
-        <v>129</v>
-      </c>
-      <c r="F68" s="61"/>
+      <c r="B68" s="64"/>
+      <c r="C68" s="65" t="s">
+        <v>81</v>
+      </c>
+      <c r="D68" s="64"/>
+      <c r="E68" s="65" t="s">
+        <v>127</v>
+      </c>
+      <c r="F68" s="66"/>
       <c r="H68" s="2">
         <v>2</v>
       </c>
@@ -3700,7 +3697,7 @@
         <v>16</v>
       </c>
       <c r="L68" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M68" s="24" t="s">
         <v>22</v>
@@ -3767,10 +3764,10 @@
         <v>16</v>
       </c>
       <c r="L70" s="49" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M70" s="26" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="71" spans="1:13" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -3785,7 +3782,7 @@
         <v>16</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F71" s="24" t="s">
         <v>37</v>
@@ -3808,18 +3805,18 @@
       <c r="F72" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="H72" s="58" t="s">
+      <c r="H72" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="I72" s="59"/>
-      <c r="J72" s="60" t="s">
-        <v>98</v>
-      </c>
-      <c r="K72" s="59"/>
-      <c r="L72" s="60" t="s">
-        <v>130</v>
-      </c>
-      <c r="M72" s="61"/>
+      <c r="I72" s="64"/>
+      <c r="J72" s="65" t="s">
+        <v>96</v>
+      </c>
+      <c r="K72" s="64"/>
+      <c r="L72" s="65" t="s">
+        <v>128</v>
+      </c>
+      <c r="M72" s="66"/>
     </row>
     <row r="73" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H73" s="18" t="s">
@@ -3853,10 +3850,10 @@
         <v>16</v>
       </c>
       <c r="L74" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M74" s="25" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="75" spans="1:13" ht="72" x14ac:dyDescent="0.3">
@@ -3871,7 +3868,7 @@
         <v>16</v>
       </c>
       <c r="L75" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M75" s="24" t="s">
         <v>30</v>
@@ -3903,26 +3900,26 @@
         <v>16</v>
       </c>
       <c r="L77" s="49" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M77" s="26" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="78" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="79" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H79" s="58" t="s">
+      <c r="H79" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="I79" s="59"/>
-      <c r="J79" s="60" t="s">
-        <v>99</v>
-      </c>
-      <c r="K79" s="59"/>
-      <c r="L79" s="60" t="s">
-        <v>132</v>
-      </c>
-      <c r="M79" s="61"/>
+      <c r="I79" s="64"/>
+      <c r="J79" s="65" t="s">
+        <v>97</v>
+      </c>
+      <c r="K79" s="64"/>
+      <c r="L79" s="65" t="s">
+        <v>130</v>
+      </c>
+      <c r="M79" s="66"/>
     </row>
     <row r="80" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H80" s="18" t="s">
@@ -3956,10 +3953,10 @@
         <v>16</v>
       </c>
       <c r="L81" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M81" s="25" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="82" spans="7:13" ht="57.6" x14ac:dyDescent="0.3">
@@ -3974,7 +3971,7 @@
         <v>16</v>
       </c>
       <c r="L82" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="M82" s="24" t="s">
         <v>37</v>
@@ -4006,26 +4003,26 @@
         <v>16</v>
       </c>
       <c r="L84" s="49" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M84" s="26" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="86" spans="7:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="87" spans="7:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H87" s="58" t="s">
+      <c r="H87" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="I87" s="59"/>
-      <c r="J87" s="60" t="s">
-        <v>101</v>
-      </c>
-      <c r="K87" s="59"/>
-      <c r="L87" s="60" t="s">
-        <v>133</v>
-      </c>
-      <c r="M87" s="61"/>
+      <c r="I87" s="64"/>
+      <c r="J87" s="65" t="s">
+        <v>99</v>
+      </c>
+      <c r="K87" s="64"/>
+      <c r="L87" s="65" t="s">
+        <v>131</v>
+      </c>
+      <c r="M87" s="66"/>
     </row>
     <row r="88" spans="7:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H88" s="18" t="s">
@@ -4059,10 +4056,10 @@
         <v>16</v>
       </c>
       <c r="L89" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M89" s="25" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="90" spans="7:13" ht="57.6" x14ac:dyDescent="0.3">
@@ -4077,10 +4074,10 @@
         <v>16</v>
       </c>
       <c r="L90" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="M90" s="24" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
     </row>
     <row r="91" spans="7:13" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -4110,26 +4107,26 @@
         <v>16</v>
       </c>
       <c r="L92" s="49" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M92" s="26" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="94" spans="7:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="95" spans="7:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H95" s="58" t="s">
+      <c r="H95" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="I95" s="59"/>
-      <c r="J95" s="60" t="s">
-        <v>103</v>
-      </c>
-      <c r="K95" s="59"/>
-      <c r="L95" s="60" t="s">
-        <v>134</v>
-      </c>
-      <c r="M95" s="61"/>
+      <c r="I95" s="64"/>
+      <c r="J95" s="65" t="s">
+        <v>101</v>
+      </c>
+      <c r="K95" s="64"/>
+      <c r="L95" s="65" t="s">
+        <v>132</v>
+      </c>
+      <c r="M95" s="66"/>
     </row>
     <row r="96" spans="7:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H96" s="18" t="s">
@@ -4163,10 +4160,10 @@
         <v>16</v>
       </c>
       <c r="L97" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M97" s="25" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="98" spans="7:13" ht="57.6" x14ac:dyDescent="0.3">
@@ -4181,7 +4178,7 @@
         <v>16</v>
       </c>
       <c r="L98" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="M98" s="24" t="s">
         <v>22</v>
@@ -4214,26 +4211,26 @@
         <v>16</v>
       </c>
       <c r="L100" s="49" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M100" s="26" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="103" spans="7:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="104" spans="7:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H104" s="58" t="s">
+      <c r="H104" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="I104" s="59"/>
-      <c r="J104" s="60" t="s">
-        <v>104</v>
-      </c>
-      <c r="K104" s="59"/>
-      <c r="L104" s="60" t="s">
-        <v>136</v>
-      </c>
-      <c r="M104" s="61"/>
+      <c r="I104" s="64"/>
+      <c r="J104" s="65" t="s">
+        <v>102</v>
+      </c>
+      <c r="K104" s="64"/>
+      <c r="L104" s="65" t="s">
+        <v>134</v>
+      </c>
+      <c r="M104" s="66"/>
     </row>
     <row r="105" spans="7:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H105" s="18" t="s">
@@ -4267,10 +4264,10 @@
         <v>16</v>
       </c>
       <c r="L106" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M106" s="25" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="107" spans="7:13" ht="57.6" x14ac:dyDescent="0.3">
@@ -4286,7 +4283,7 @@
         <v>16</v>
       </c>
       <c r="L107" s="30" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M107" s="31" t="s">
         <v>30</v>
@@ -4319,26 +4316,26 @@
         <v>16</v>
       </c>
       <c r="L109" s="49" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M109" s="26" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="112" spans="7:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="113" spans="7:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H113" s="58" t="s">
+      <c r="H113" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="I113" s="59"/>
-      <c r="J113" s="60" t="s">
-        <v>107</v>
-      </c>
-      <c r="K113" s="59"/>
-      <c r="L113" s="60" t="s">
-        <v>137</v>
-      </c>
-      <c r="M113" s="61"/>
+      <c r="I113" s="64"/>
+      <c r="J113" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="K113" s="64"/>
+      <c r="L113" s="65" t="s">
+        <v>135</v>
+      </c>
+      <c r="M113" s="66"/>
     </row>
     <row r="114" spans="7:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H114" s="18" t="s">
@@ -4372,10 +4369,10 @@
         <v>16</v>
       </c>
       <c r="L115" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M115" s="25" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="116" spans="7:13" ht="57.6" x14ac:dyDescent="0.3">
@@ -4390,7 +4387,7 @@
         <v>16</v>
       </c>
       <c r="L116" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M116" s="24" t="s">
         <v>37</v>
@@ -4423,26 +4420,26 @@
         <v>16</v>
       </c>
       <c r="L118" s="49" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M118" s="26" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="120" spans="7:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="121" spans="7:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H121" s="58" t="s">
+      <c r="H121" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="I121" s="59"/>
-      <c r="J121" s="60" t="s">
-        <v>85</v>
-      </c>
-      <c r="K121" s="59"/>
-      <c r="L121" s="60" t="s">
-        <v>139</v>
-      </c>
-      <c r="M121" s="61"/>
+      <c r="I121" s="64"/>
+      <c r="J121" s="65" t="s">
+        <v>84</v>
+      </c>
+      <c r="K121" s="64"/>
+      <c r="L121" s="65" t="s">
+        <v>137</v>
+      </c>
+      <c r="M121" s="66"/>
     </row>
     <row r="122" spans="7:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H122" s="18" t="s">
@@ -4523,18 +4520,18 @@
     </row>
     <row r="128" spans="7:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="129" spans="8:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H129" s="58" t="s">
+      <c r="H129" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="I129" s="59"/>
-      <c r="J129" s="60" t="s">
-        <v>140</v>
-      </c>
-      <c r="K129" s="59"/>
-      <c r="L129" s="62" t="s">
-        <v>111</v>
-      </c>
-      <c r="M129" s="63"/>
+      <c r="I129" s="64"/>
+      <c r="J129" s="65" t="s">
+        <v>138</v>
+      </c>
+      <c r="K129" s="64"/>
+      <c r="L129" s="67" t="s">
+        <v>109</v>
+      </c>
+      <c r="M129" s="68"/>
     </row>
     <row r="130" spans="8:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H130" s="18" t="s">
@@ -4568,10 +4565,10 @@
         <v>16</v>
       </c>
       <c r="L131" s="22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M131" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="132" spans="8:13" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -4594,18 +4591,18 @@
     </row>
     <row r="135" spans="8:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="136" spans="8:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H136" s="65" t="s">
+      <c r="H136" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="I136" s="66"/>
-      <c r="J136" s="67" t="s">
-        <v>141</v>
-      </c>
-      <c r="K136" s="66"/>
-      <c r="L136" s="68" t="s">
-        <v>113</v>
-      </c>
-      <c r="M136" s="69"/>
+      <c r="I136" s="59"/>
+      <c r="J136" s="60" t="s">
+        <v>139</v>
+      </c>
+      <c r="K136" s="59"/>
+      <c r="L136" s="61" t="s">
+        <v>111</v>
+      </c>
+      <c r="M136" s="62"/>
     </row>
     <row r="137" spans="8:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H137" s="18" t="s">
@@ -4639,10 +4636,10 @@
         <v>16</v>
       </c>
       <c r="L138" s="49" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M138" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="139" spans="8:13" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -4657,7 +4654,7 @@
         <v>16</v>
       </c>
       <c r="L139" s="8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="M139" s="26" t="s">
         <v>26</v>
@@ -4665,15 +4662,87 @@
     </row>
   </sheetData>
   <mergeCells count="102">
-    <mergeCell ref="H136:I136"/>
-    <mergeCell ref="J136:K136"/>
-    <mergeCell ref="L136:M136"/>
-    <mergeCell ref="H121:I121"/>
-    <mergeCell ref="J121:K121"/>
-    <mergeCell ref="L121:M121"/>
-    <mergeCell ref="H129:I129"/>
-    <mergeCell ref="J129:K129"/>
-    <mergeCell ref="L129:M129"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="L38:M38"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="L44:M44"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="J52:K52"/>
+    <mergeCell ref="L52:M52"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="J46:K46"/>
+    <mergeCell ref="L46:M46"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="E68:F68"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="J58:K58"/>
+    <mergeCell ref="L58:M58"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="H72:I72"/>
+    <mergeCell ref="J72:K72"/>
+    <mergeCell ref="L72:M72"/>
+    <mergeCell ref="H79:I79"/>
+    <mergeCell ref="J79:K79"/>
+    <mergeCell ref="L79:M79"/>
+    <mergeCell ref="H65:I65"/>
+    <mergeCell ref="J65:K65"/>
+    <mergeCell ref="L65:M65"/>
     <mergeCell ref="H104:I104"/>
     <mergeCell ref="J104:K104"/>
     <mergeCell ref="L104:M104"/>
@@ -4686,87 +4755,15 @@
     <mergeCell ref="H95:I95"/>
     <mergeCell ref="J95:K95"/>
     <mergeCell ref="L95:M95"/>
-    <mergeCell ref="H72:I72"/>
-    <mergeCell ref="J72:K72"/>
-    <mergeCell ref="L72:M72"/>
-    <mergeCell ref="H79:I79"/>
-    <mergeCell ref="J79:K79"/>
-    <mergeCell ref="L79:M79"/>
-    <mergeCell ref="H65:I65"/>
-    <mergeCell ref="J65:K65"/>
-    <mergeCell ref="L65:M65"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="E68:F68"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="J58:K58"/>
-    <mergeCell ref="L58:M58"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="J52:K52"/>
-    <mergeCell ref="L52:M52"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="J46:K46"/>
-    <mergeCell ref="L46:M46"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="J38:K38"/>
-    <mergeCell ref="L38:M38"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="L44:M44"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="H136:I136"/>
+    <mergeCell ref="J136:K136"/>
+    <mergeCell ref="L136:M136"/>
+    <mergeCell ref="H121:I121"/>
+    <mergeCell ref="J121:K121"/>
+    <mergeCell ref="L121:M121"/>
+    <mergeCell ref="H129:I129"/>
+    <mergeCell ref="J129:K129"/>
+    <mergeCell ref="L129:M129"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>